<commit_message>
Se agregan los reportes asociados a cometidos
</commit_message>
<xml_diff>
--- a/App.Web/App_Data/CAIGG.xlsx
+++ b/App.Web/App_Data/CAIGG.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GestionProcesos\Reportes\Cometidos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GestionProcesos\SourceNew\App.Web\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7605"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="20490" windowHeight="7605"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$I$1:$W$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$W$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -431,15 +431,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="33" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,54 +480,54 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="Q1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="I1:W1"/>
+  <autoFilter ref="A1:W1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
30-09-2020 -modificaciones en formato de resoluciones -se agregan campos nuevos en reporte caigg -se modifica metodo que carga reporte caigg -se crean campoos nuevos en las tareas de abasteciemiento -se agrega separador de miles a monto de viatico en resolucion -se agrega separador de miles en las vistas que se muestra el compromiso cdp
</commit_message>
<xml_diff>
--- a/App.Web/App_Data/CAIGG.xlsx
+++ b/App.Web/App_Data/CAIGG.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GestionProcesos\SourceNew\App.Web\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GestionProcesos\Reportes\Cometidos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="20490" windowHeight="7605"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="20490" windowHeight="7605"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$W$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$AB$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Subsecretaría</t>
   </si>
@@ -93,6 +93,21 @@
   </si>
   <si>
     <t>Estado del pago</t>
+  </si>
+  <si>
+    <t>Clase de Pasaje</t>
+  </si>
+  <si>
+    <t>Forma de Adquisición del pasaje</t>
+  </si>
+  <si>
+    <t>Fecha de Adquisición</t>
+  </si>
+  <si>
+    <t>Fecha del vuelo</t>
+  </si>
+  <si>
+    <t>ID Orden de compra</t>
   </si>
 </sst>
 </file>
@@ -431,34 +446,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="44.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="52.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="50.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="48.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="33" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" customWidth="1"/>
+    <col min="13" max="13" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="50.5703125" customWidth="1"/>
+    <col min="16" max="16" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="48.5703125" customWidth="1"/>
+    <col min="18" max="19" width="19.5703125" customWidth="1"/>
+    <col min="20" max="20" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="33" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,41 +515,56 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W1"/>
+  <autoFilter ref="A1:AB1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>